<commit_message>
update docs for `nexial.lastOutputPath`
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/rdbms/artifact/script/rdbms.xlsx
+++ b/examples/rdbms/artifact/script/rdbms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/examples/rdbms/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463FD9B-5C18-3D43-9C88-7B3FFF864377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50697427-00E6-EC49-979F-0A900D9B8094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13340" yWindow="460" windowWidth="36340" windowHeight="21140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="570">
   <si>
     <t>description</t>
   </si>
@@ -1780,6 +1780,12 @@
   </si>
   <si>
     <t>[TEXT(${example1.outFiles}) =&gt; replace(\,,\n)]</t>
+  </si>
+  <si>
+    <t>${nexial.lastOutputPath}</t>
+  </si>
+  <si>
+    <t>${nexial.lastOutputLink}</t>
   </si>
 </sst>
 </file>
@@ -4406,7 +4412,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4683,9 +4689,15 @@
     <row r="10" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="C10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>568</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -4700,9 +4712,15 @@
     <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>569</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>

</xml_diff>